<commit_message>
finished working on graphs before the lecture.
</commit_message>
<xml_diff>
--- a/admin/Project_task_planning.xlsx
+++ b/admin/Project_task_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data challenge 3\project_1\data_challenge_3_project\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010D87E2-625A-4714-AA15-959D8F2A9074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA771D3F-2066-48AE-9C74-0F83BDF86F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{7A7D0F82-19BC-4D4C-8900-8B53D9DA9A08}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>W1</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Project Plan</t>
   </si>
   <si>
-    <t>Report</t>
-  </si>
-  <si>
     <t>Presentation</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>24/10/2022 30/10/2022</t>
   </si>
   <si>
-    <t>31/10/2022 03/11/2022</t>
-  </si>
-  <si>
     <t>CB: preprocessing of cancelled orders, CP: start of NLP, aggregated dataset</t>
   </si>
   <si>
@@ -110,7 +104,16 @@
     <t>W8</t>
   </si>
   <si>
-    <t>Both: finish feature selection, evaluate models and start generating material for the report.</t>
+    <t>Both: finish feature selection</t>
+  </si>
+  <si>
+    <t>W7</t>
+  </si>
+  <si>
+    <t>Finish model evaluation, write report</t>
+  </si>
+  <si>
+    <t>31/10/2022 6/11/2022</t>
   </si>
 </sst>
 </file>
@@ -161,7 +164,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,16 +317,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +644,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,10 +670,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -678,10 +681,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -689,10 +692,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -700,10 +703,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -711,43 +714,43 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="16" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="19">
+        <v>44876</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added readme.txt to explain the project flow.
</commit_message>
<xml_diff>
--- a/admin/Project_task_planning.xlsx
+++ b/admin/Project_task_planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data challenge 3\project_1\data_challenge_3_project\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA771D3F-2066-48AE-9C74-0F83BDF86F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A5EFDB-EF23-407B-A2EF-18022980A0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{7A7D0F82-19BC-4D4C-8900-8B53D9DA9A08}"/>
+    <workbookView xWindow="3696" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{7A7D0F82-19BC-4D4C-8900-8B53D9DA9A08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>W1</t>
   </si>
@@ -114,6 +114,54 @@
   </si>
   <si>
     <t>31/10/2022 6/11/2022</t>
+  </si>
+  <si>
+    <t>Final Division</t>
+  </si>
+  <si>
+    <t>Preprocessing</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>NLP</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Time series</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>RFM</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>Wrappers</t>
+  </si>
+  <si>
+    <t>Dimensionality Reduction</t>
+  </si>
+  <si>
+    <t>Modelling</t>
+  </si>
+  <si>
+    <t>Error analysis</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Responsible</t>
   </si>
 </sst>
 </file>
@@ -342,6 +390,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EDDC984A-63DF-41B5-858F-254A388B28C1}" name="Table2" displayName="Table2" ref="A11:B22" totalsRowShown="0">
+  <autoFilter ref="A11:B22" xr:uid="{EDDC984A-63DF-41B5-858F-254A388B28C1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A3D1C2ED-221F-4EE8-B5F1-C76940B36D66}" name="Final Division"/>
+    <tableColumn id="2" xr3:uid="{EE3FE9B3-6007-4C95-8F3B-1D6D9917ED66}" name="Responsible"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -641,15 +700,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F381BE3B-6E13-4D3B-8310-A17B56C0CCA2}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="100.33203125" customWidth="1"/>
   </cols>
@@ -757,19 +816,111 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
       <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>